<commit_message>
Definition of Rounds 1 - 4
</commit_message>
<xml_diff>
--- a/Einschatzung_Spieler_Runden.xlsx
+++ b/Einschatzung_Spieler_Runden.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\node.js\virtual7jeopardy\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\virtual7jeopardy\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="68">
   <si>
     <t>Michael Augustin</t>
   </si>
@@ -166,13 +166,76 @@
   </si>
   <si>
     <t>Runde 3</t>
+  </si>
+  <si>
+    <t>Runde 4</t>
+  </si>
+  <si>
+    <t>App Icons</t>
+  </si>
+  <si>
+    <t>Unix Commands</t>
+  </si>
+  <si>
+    <t>Finale</t>
+  </si>
+  <si>
+    <t>Who am I / Who are they</t>
+  </si>
+  <si>
+    <t>Oracle Ports</t>
+  </si>
+  <si>
+    <t>Miram</t>
+  </si>
+  <si>
+    <t>Tobi</t>
+  </si>
+  <si>
+    <t>Cipi</t>
+  </si>
+  <si>
+    <t>Markus</t>
+  </si>
+  <si>
+    <t>Jochen</t>
+  </si>
+  <si>
+    <t>Michael</t>
+  </si>
+  <si>
+    <t>Roger</t>
+  </si>
+  <si>
+    <t>Björn</t>
+  </si>
+  <si>
+    <t>Roland</t>
+  </si>
+  <si>
+    <t>Marco</t>
+  </si>
+  <si>
+    <t>Anton</t>
+  </si>
+  <si>
+    <t>Adrian</t>
+  </si>
+  <si>
+    <t>Christian</t>
+  </si>
+  <si>
+    <t>Arkadi</t>
+  </si>
+  <si>
+    <t>???</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -197,6 +260,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -234,19 +305,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="4"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
+    <cellStyle name="Erklärender Text" xfId="4" builtinId="53"/>
     <cellStyle name="Gut" xfId="1" builtinId="26"/>
     <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Schlecht" xfId="2" builtinId="27"/>
@@ -531,7 +605,7 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection sqref="A1:D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -679,10 +753,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J20"/>
+  <dimension ref="A1:K39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -692,7 +766,7 @@
     <col min="11" max="11" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>16</v>
       </c>
@@ -709,8 +783,8 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>19</v>
       </c>
       <c r="B2" s="1"/>
@@ -723,9 +797,12 @@
       <c r="J2" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="K2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
         <v>21</v>
       </c>
       <c r="B3" s="1"/>
@@ -738,9 +815,12 @@
       <c r="J3" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="K3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
         <v>22</v>
       </c>
       <c r="B4" s="1"/>
@@ -753,9 +833,12 @@
       <c r="J4" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="K4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
         <v>23</v>
       </c>
       <c r="B5" s="1"/>
@@ -768,9 +851,12 @@
       <c r="J5" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="K5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
         <v>24</v>
       </c>
       <c r="B6" s="2"/>
@@ -784,8 +870,8 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
         <v>25</v>
       </c>
       <c r="B7" s="3"/>
@@ -799,8 +885,8 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
         <v>26</v>
       </c>
       <c r="B8" s="1"/>
@@ -808,8 +894,8 @@
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
         <v>27</v>
       </c>
       <c r="B9" s="3"/>
@@ -820,8 +906,8 @@
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
         <v>28</v>
       </c>
       <c r="B10" s="1"/>
@@ -834,8 +920,11 @@
       <c r="J10" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>29</v>
       </c>
@@ -849,8 +938,11 @@
       <c r="J11" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K11" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>30</v>
       </c>
@@ -864,9 +956,12 @@
       <c r="J12" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="K12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
         <v>31</v>
       </c>
       <c r="B13" s="3"/>
@@ -879,8 +974,11 @@
       <c r="J13" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K13" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>32</v>
       </c>
@@ -889,13 +987,13 @@
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
       <c r="I14" t="s">
-        <v>44</v>
-      </c>
-      <c r="J14" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>33</v>
       </c>
@@ -910,8 +1008,8 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
         <v>34</v>
       </c>
       <c r="B16" s="1"/>
@@ -919,8 +1017,8 @@
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
         <v>35</v>
       </c>
       <c r="B17" s="1"/>
@@ -931,7 +1029,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>36</v>
       </c>
@@ -939,24 +1037,199 @@
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="I18" t="s">
+        <v>34</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K18" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
         <v>38</v>
       </c>
       <c r="B19" s="3"/>
       <c r="C19" s="1"/>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="I19" t="s">
+        <v>30</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K19" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
         <v>37</v>
       </c>
       <c r="B20" s="3"/>
       <c r="C20" s="1"/>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
+      <c r="I20" t="s">
+        <v>38</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K20" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I21" t="s">
+        <v>37</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K21" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I22" t="s">
+        <v>33</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I23" t="s">
+        <v>44</v>
+      </c>
+      <c r="J23" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I25" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I26" t="s">
+        <v>40</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K26" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I27" t="s">
+        <v>48</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K27" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I28" t="s">
+        <v>24</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K28" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I29" t="s">
+        <v>31</v>
+      </c>
+      <c r="J29" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K29" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I30" t="s">
+        <v>49</v>
+      </c>
+      <c r="J30" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I31" t="s">
+        <v>33</v>
+      </c>
+      <c r="J31" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="33" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I33" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="34" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I34" t="s">
+        <v>35</v>
+      </c>
+      <c r="J34" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K34" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="35" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I35" t="s">
+        <v>40</v>
+      </c>
+      <c r="J35" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="36" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I36" t="s">
+        <v>33</v>
+      </c>
+      <c r="J36" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="37" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I37" t="s">
+        <v>30</v>
+      </c>
+      <c r="J37" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="38" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I38" t="s">
+        <v>51</v>
+      </c>
+      <c r="J38" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="39" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I39" t="s">
+        <v>52</v>
+      </c>
+      <c r="J39" s="3" t="s">
+        <v>16</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>